<commit_message>
Main Project File Updated.
</commit_message>
<xml_diff>
--- a/Pre Research Works/match.xlsx
+++ b/Pre Research Works/match.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •']</t>
+          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •']</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], []</t>
+          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], []</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
+          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], []</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], []</t>
+          <t>['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards'], ['activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •'], ['activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •', 'activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], ['objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •'], []</t>
         </is>
       </c>
     </row>

</xml_diff>